<commit_message>
gestion du lvl up + crash inconnu a des moments
</commit_message>
<xml_diff>
--- a/Analyse/chiffres.xlsx
+++ b/Analyse/chiffres.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Suchgamewow\Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\suchGame\Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -736,35 +736,35 @@
       </c>
       <c r="H3" s="22">
         <f t="shared" ref="H3:J12" ca="1" si="0" xml:space="preserve"> $E3 + $E3 * (RANDBETWEEN(1,$H$13) - $H$13/2) / 100</f>
-        <v>103.88</v>
+        <v>93.1</v>
       </c>
       <c r="I3" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>104.86</v>
+        <v>95.06</v>
       </c>
       <c r="J3" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>106.82</v>
+        <v>96.04</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" ref="K3:M12" ca="1" si="1" xml:space="preserve"> $F3 + $F3 * (RANDBETWEEN(1,$K$13) -$K$13/2) / 100</f>
-        <v>44.44</v>
+        <v>43.12</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44.88</v>
+        <v>43.56</v>
       </c>
       <c r="M3" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44.88</v>
+        <v>45.76</v>
       </c>
       <c r="N3" s="23">
         <f t="shared" ref="N3:N12" ca="1" si="2">SUM(H3:J3)/COUNT(H3:J3)</f>
-        <v>105.18666666666667</v>
+        <v>94.733333333333334</v>
       </c>
       <c r="O3" s="23">
         <f t="shared" ref="O3:O12" ca="1" si="3">SUM(K3:M3)/COUNT(K3:M3)</f>
-        <v>44.733333333333327</v>
+        <v>44.146666666666668</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -795,23 +795,23 @@
       </c>
       <c r="H4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>107.12</v>
+        <v>112.32</v>
       </c>
       <c r="I4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>98.8</v>
+        <v>113.36</v>
       </c>
       <c r="J4" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>112.32</v>
+        <v>104</v>
       </c>
       <c r="K4" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>49.92</v>
+        <v>48.96</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>46.08</v>
+        <v>46.56</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -819,11 +819,11 @@
       </c>
       <c r="N4" s="26">
         <f t="shared" ca="1" si="2"/>
-        <v>106.08</v>
+        <v>109.89333333333333</v>
       </c>
       <c r="O4" s="26">
         <f t="shared" ca="1" si="3"/>
-        <v>48.32</v>
+        <v>48.160000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -854,23 +854,23 @@
       </c>
       <c r="H5" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>111.1</v>
+        <v>100.1</v>
       </c>
       <c r="I5" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>114.4</v>
+        <v>115.5</v>
       </c>
       <c r="J5" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>110</v>
+        <v>113.3</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>54.6</v>
+        <v>52</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>50.96</v>
+        <v>52.52</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ca="1" si="1"/>
@@ -878,11 +878,11 @@
       </c>
       <c r="N5" s="23">
         <f t="shared" ca="1" si="2"/>
-        <v>111.83333333333333</v>
+        <v>109.63333333333333</v>
       </c>
       <c r="O5" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>52</v>
+        <v>51.653333333333336</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -913,19 +913,19 @@
       </c>
       <c r="H6" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>111.36</v>
+        <v>118.32</v>
       </c>
       <c r="I6" s="25">
         <f t="shared" ca="1" si="0"/>
+        <v>117.16</v>
+      </c>
+      <c r="J6" s="25">
+        <f t="shared" ca="1" si="0"/>
         <v>119.48</v>
       </c>
-      <c r="J6" s="25">
-        <f t="shared" ca="1" si="0"/>
-        <v>110.2</v>
-      </c>
       <c r="K6" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>54.88</v>
+        <v>53.76</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -933,15 +933,15 @@
       </c>
       <c r="M6" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>55.44</v>
+        <v>58.8</v>
       </c>
       <c r="N6" s="26">
         <f t="shared" ca="1" si="2"/>
-        <v>113.68</v>
+        <v>118.32</v>
       </c>
       <c r="O6" s="26">
         <f t="shared" ca="1" si="3"/>
-        <v>56</v>
+        <v>56.74666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -972,35 +972,35 @@
       </c>
       <c r="H7" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>126.88</v>
+        <v>118.34</v>
       </c>
       <c r="I7" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>124.44</v>
+        <v>115.9</v>
       </c>
       <c r="J7" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>134.19999999999999</v>
+        <v>130.54</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>58.2</v>
+        <v>58.8</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>62.4</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>57.6</v>
+        <v>62.4</v>
       </c>
       <c r="N7" s="23">
         <f t="shared" ca="1" si="2"/>
-        <v>128.50666666666666</v>
+        <v>121.59333333333332</v>
       </c>
       <c r="O7" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>58.6</v>
+        <v>61.199999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1031,35 +1031,35 @@
       </c>
       <c r="H8" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>121.6</v>
+        <v>124.16</v>
       </c>
       <c r="I8" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>134.4</v>
+        <v>120.32</v>
       </c>
       <c r="J8" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>129.28</v>
+        <v>117.76</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" ca="1" si="1"/>
+        <v>61.44</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" ca="1" si="1"/>
         <v>66.56</v>
       </c>
-      <c r="L8" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>65.92</v>
-      </c>
       <c r="M8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>64.64</v>
       </c>
       <c r="N8" s="26">
         <f t="shared" ca="1" si="2"/>
-        <v>128.42666666666665</v>
+        <v>120.74666666666667</v>
       </c>
       <c r="O8" s="26">
         <f t="shared" ca="1" si="3"/>
-        <v>65.493333333333339</v>
+        <v>64.213333333333324</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1090,35 +1090,35 @@
       </c>
       <c r="H9" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>127.3</v>
+        <v>123.28</v>
       </c>
       <c r="I9" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>136.68</v>
+        <v>134</v>
       </c>
       <c r="J9" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>146.06</v>
+        <v>124.62</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>70.72</v>
+        <v>68</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>71.400000000000006</v>
+        <v>65.28</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>70.040000000000006</v>
+        <v>65.959999999999994</v>
       </c>
       <c r="N9" s="23">
         <f t="shared" ca="1" si="2"/>
-        <v>136.68</v>
+        <v>127.3</v>
       </c>
       <c r="O9" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>70.720000000000013</v>
+        <v>66.413333333333341</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1149,35 +1149,35 @@
       </c>
       <c r="H10" s="25">
         <f t="shared" ca="1" si="0"/>
+        <v>128.80000000000001</v>
+      </c>
+      <c r="I10" s="25">
+        <f t="shared" ca="1" si="0"/>
         <v>145.6</v>
       </c>
-      <c r="I10" s="25">
-        <f t="shared" ca="1" si="0"/>
-        <v>140</v>
-      </c>
       <c r="J10" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>128.80000000000001</v>
+        <v>149.80000000000001</v>
       </c>
       <c r="K10" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>74.16</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="M10" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>69.84</v>
+        <v>69.12</v>
       </c>
       <c r="N10" s="26">
         <f t="shared" ca="1" si="2"/>
-        <v>138.13333333333335</v>
+        <v>141.4</v>
       </c>
       <c r="O10" s="26">
         <f t="shared" ca="1" si="3"/>
-        <v>72</v>
+        <v>73.44</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1208,35 +1208,35 @@
       </c>
       <c r="H11" s="22">
         <f t="shared" ca="1" si="0"/>
+        <v>138.69999999999999</v>
+      </c>
+      <c r="I11" s="22">
+        <f t="shared" ca="1" si="0"/>
         <v>159.13999999999999</v>
       </c>
-      <c r="I11" s="22">
-        <f t="shared" ca="1" si="0"/>
-        <v>159.13999999999999</v>
-      </c>
       <c r="J11" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>151.84</v>
+        <v>147.46</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" ca="1" si="1"/>
+        <v>76.760000000000005</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" ca="1" si="1"/>
         <v>75.239999999999995</v>
       </c>
-      <c r="L11" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>78.28</v>
-      </c>
       <c r="M11" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>75.239999999999995</v>
+        <v>76</v>
       </c>
       <c r="N11" s="23">
         <f t="shared" ca="1" si="2"/>
-        <v>156.70666666666668</v>
+        <v>148.43333333333331</v>
       </c>
       <c r="O11" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>76.25333333333333</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1267,35 +1267,35 @@
       </c>
       <c r="H12" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>158.08000000000001</v>
+        <v>147.44</v>
       </c>
       <c r="I12" s="25">
         <f t="shared" ca="1" si="0"/>
+        <v>159.6</v>
+      </c>
+      <c r="J12" s="25">
+        <f t="shared" ca="1" si="0"/>
         <v>165.68</v>
       </c>
-      <c r="J12" s="25">
-        <f t="shared" ca="1" si="0"/>
-        <v>138.32</v>
-      </c>
       <c r="K12" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>80.8</v>
+        <v>80</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>77.599999999999994</v>
+        <v>83.2</v>
       </c>
       <c r="M12" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>78.400000000000006</v>
+        <v>79.2</v>
       </c>
       <c r="N12" s="26">
         <f t="shared" ca="1" si="2"/>
-        <v>154.02666666666667</v>
+        <v>157.57333333333332</v>
       </c>
       <c r="O12" s="26">
         <f t="shared" ca="1" si="3"/>
-        <v>78.933333333333323</v>
+        <v>80.8</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1320,39 +1320,39 @@
       </c>
       <c r="H14" s="14">
         <f t="shared" ref="H14:M14" ca="1" si="8">SUM(H3:H12)/COUNT(H3:H12)</f>
-        <v>127.20599999999999</v>
+        <v>120.45599999999999</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" ca="1" si="8"/>
-        <v>129.78799999999998</v>
+        <v>127.56399999999999</v>
       </c>
       <c r="J14" s="14">
         <f t="shared" ca="1" si="8"/>
-        <v>126.78399999999996</v>
+        <v>126.86800000000001</v>
       </c>
       <c r="K14" s="14">
         <f t="shared" ca="1" si="8"/>
-        <v>62.736000000000004</v>
+        <v>61.843999999999994</v>
       </c>
       <c r="L14" s="14">
         <f t="shared" ca="1" si="8"/>
-        <v>62.696000000000005</v>
+        <v>62.860000000000014</v>
       </c>
       <c r="M14" s="14">
         <f t="shared" ca="1" si="8"/>
-        <v>61.484000000000002</v>
+        <v>62.128</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H15" s="14">
         <f ca="1">SUM(H14:J14) / COUNT(H14:J14)</f>
-        <v>127.92599999999997</v>
+        <v>124.96266666666666</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14">
         <f ca="1">SUM(K14:M14) / COUNT(K14:M14)</f>
-        <v>62.305333333333344</v>
+        <v>62.277333333333331</v>
       </c>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
@@ -1420,35 +1420,35 @@
       </c>
       <c r="G18" s="23">
         <f t="shared" ref="G18:I27" ca="1" si="9" xml:space="preserve"> $D18 + $D18 * (RANDBETWEEN(1,$G$28) - $G$28/2) / 100</f>
-        <v>81.599999999999994</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="H18" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>78.400000000000006</v>
+        <v>85.6</v>
       </c>
       <c r="I18" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>73.599999999999994</v>
+        <v>82.4</v>
       </c>
       <c r="J18" s="23">
         <f t="shared" ref="J18:L27" ca="1" si="10" xml:space="preserve"> $E18 + $E18 * (RANDBETWEEN(1,$G$28) - $G$28/2) / 100</f>
-        <v>27.6</v>
+        <v>29.1</v>
       </c>
       <c r="K18" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>31.5</v>
+        <v>27.3</v>
       </c>
       <c r="L18" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>30.9</v>
+        <v>27.9</v>
       </c>
       <c r="M18" s="23">
         <f t="shared" ref="M18:M27" ca="1" si="11">SUM(G18:I18)/COUNT(G18:I18)</f>
-        <v>77.86666666666666</v>
+        <v>82.13333333333334</v>
       </c>
       <c r="N18" s="23">
         <f t="shared" ref="N18:N27" ca="1" si="12">SUM(J18:L18)/COUNT(J18:L18)</f>
-        <v>30</v>
+        <v>28.100000000000005</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1477,35 +1477,35 @@
       </c>
       <c r="G19" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>97.85</v>
+        <v>89.3</v>
       </c>
       <c r="H19" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>91.2</v>
+        <v>104.5</v>
       </c>
       <c r="I19" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>89.3</v>
+        <v>87.4</v>
       </c>
       <c r="J19" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>41</v>
+        <v>40.18</v>
       </c>
       <c r="K19" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>45.1</v>
+        <v>44.28</v>
       </c>
       <c r="L19" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>43.87</v>
+        <v>37.31</v>
       </c>
       <c r="M19" s="26">
         <f t="shared" ca="1" si="11"/>
-        <v>92.783333333333346</v>
+        <v>93.733333333333348</v>
       </c>
       <c r="N19" s="26">
         <f t="shared" ca="1" si="12"/>
-        <v>43.323333333333331</v>
+        <v>40.590000000000003</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1534,11 +1534,11 @@
       </c>
       <c r="G20" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>113.3</v>
+        <v>104.5</v>
       </c>
       <c r="H20" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>110</v>
+        <v>112.2</v>
       </c>
       <c r="I20" s="23">
         <f t="shared" ca="1" si="9"/>
@@ -1546,23 +1546,23 @@
       </c>
       <c r="J20" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>51.3</v>
+        <v>58.32</v>
       </c>
       <c r="K20" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>56.7</v>
+        <v>59.4</v>
       </c>
       <c r="L20" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>50.22</v>
+        <v>54</v>
       </c>
       <c r="M20" s="23">
         <f t="shared" ca="1" si="11"/>
-        <v>108.53333333333335</v>
+        <v>106.33333333333333</v>
       </c>
       <c r="N20" s="23">
         <f t="shared" ca="1" si="12"/>
-        <v>52.74</v>
+        <v>57.24</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1591,35 +1591,35 @@
       </c>
       <c r="G21" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>135</v>
+        <v>117.5</v>
       </c>
       <c r="H21" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>130</v>
+        <v>127.5</v>
       </c>
       <c r="I21" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>120</v>
+        <v>127.5</v>
       </c>
       <c r="J21" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>72.36</v>
+        <v>71.02</v>
       </c>
       <c r="K21" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>73.03</v>
+        <v>68.34</v>
       </c>
       <c r="L21" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>64.989999999999995</v>
+        <v>73.7</v>
       </c>
       <c r="M21" s="26">
         <f t="shared" ca="1" si="11"/>
-        <v>128.33333333333334</v>
+        <v>124.16666666666667</v>
       </c>
       <c r="N21" s="26">
         <f t="shared" ca="1" si="12"/>
-        <v>70.126666666666665</v>
+        <v>71.02</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1648,35 +1648,35 @@
       </c>
       <c r="G22" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>127.4</v>
+        <v>130.19999999999999</v>
       </c>
       <c r="H22" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>149.80000000000001</v>
+        <v>128.80000000000001</v>
       </c>
       <c r="I22" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>145.6</v>
+        <v>133</v>
       </c>
       <c r="J22" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>78.400000000000006</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="K22" s="23">
         <f t="shared" ca="1" si="10"/>
+        <v>73.599999999999994</v>
+      </c>
+      <c r="L22" s="23">
+        <f t="shared" ca="1" si="10"/>
         <v>83.2</v>
-      </c>
-      <c r="L22" s="23">
-        <f t="shared" ca="1" si="10"/>
-        <v>72.8</v>
       </c>
       <c r="M22" s="23">
         <f t="shared" ca="1" si="11"/>
-        <v>140.93333333333337</v>
+        <v>130.66666666666666</v>
       </c>
       <c r="N22" s="23">
         <f t="shared" ca="1" si="12"/>
-        <v>78.13333333333334</v>
+        <v>79.466666666666654</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1705,35 +1705,35 @@
       </c>
       <c r="G23" s="26">
         <f t="shared" ca="1" si="9"/>
+        <v>155</v>
+      </c>
+      <c r="H23" s="26">
+        <f t="shared" ca="1" si="9"/>
         <v>144.15</v>
       </c>
-      <c r="H23" s="26">
-        <f t="shared" ca="1" si="9"/>
-        <v>164.3</v>
-      </c>
       <c r="I23" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>165.85</v>
+        <v>158.1</v>
       </c>
       <c r="J23" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>94.86</v>
+        <v>100.44</v>
       </c>
       <c r="K23" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>99.51</v>
+        <v>95.79</v>
       </c>
       <c r="L23" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>95.79</v>
+        <v>92.07</v>
       </c>
       <c r="M23" s="26">
         <f t="shared" ca="1" si="11"/>
-        <v>158.10000000000002</v>
+        <v>152.41666666666666</v>
       </c>
       <c r="N23" s="26">
         <f t="shared" ca="1" si="12"/>
-        <v>96.720000000000013</v>
+        <v>96.100000000000009</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1762,35 +1762,35 @@
       </c>
       <c r="G24" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>170</v>
+        <v>159.80000000000001</v>
       </c>
       <c r="H24" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>166.6</v>
+        <v>171.7</v>
       </c>
       <c r="I24" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>185.3</v>
+        <v>168.3</v>
       </c>
       <c r="J24" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>108.12</v>
+        <v>106</v>
       </c>
       <c r="K24" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>112.36</v>
+        <v>99.64</v>
       </c>
       <c r="L24" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>103.88</v>
+        <v>116.6</v>
       </c>
       <c r="M24" s="23">
         <f t="shared" ca="1" si="11"/>
-        <v>173.9666666666667</v>
+        <v>166.6</v>
       </c>
       <c r="N24" s="23">
         <f t="shared" ca="1" si="12"/>
-        <v>108.12</v>
+        <v>107.41333333333334</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -1823,31 +1823,31 @@
       </c>
       <c r="H25" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>196.1</v>
+        <v>190.55</v>
       </c>
       <c r="I25" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>196.1</v>
+        <v>177.6</v>
       </c>
       <c r="J25" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>119</v>
+        <v>121.38</v>
       </c>
       <c r="K25" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>120.19</v>
+        <v>116.62</v>
       </c>
       <c r="L25" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>115.43</v>
+        <v>123.76</v>
       </c>
       <c r="M25" s="26">
         <f t="shared" ca="1" si="11"/>
-        <v>188.08333333333334</v>
+        <v>180.06666666666669</v>
       </c>
       <c r="N25" s="26">
         <f t="shared" ca="1" si="12"/>
-        <v>118.20666666666666</v>
+        <v>120.58666666666666</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1876,23 +1876,23 @@
       </c>
       <c r="G26" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="H26" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I26" s="23">
         <f t="shared" ca="1" si="9"/>
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="J26" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>138.6</v>
+        <v>142.56</v>
       </c>
       <c r="K26" s="23">
         <f t="shared" ca="1" si="10"/>
-        <v>138.6</v>
+        <v>132</v>
       </c>
       <c r="L26" s="23">
         <f t="shared" ca="1" si="10"/>
@@ -1900,11 +1900,11 @@
       </c>
       <c r="M26" s="23">
         <f t="shared" ca="1" si="11"/>
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="N26" s="23">
         <f t="shared" ca="1" si="12"/>
-        <v>137.72</v>
+        <v>136.84</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -1933,35 +1933,35 @@
       </c>
       <c r="G27" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>221.45</v>
+        <v>215</v>
       </c>
       <c r="H27" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>227.9</v>
+        <v>217.15</v>
       </c>
       <c r="I27" s="26">
         <f t="shared" ca="1" si="9"/>
-        <v>215</v>
+        <v>225.75</v>
       </c>
       <c r="J27" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>153.69999999999999</v>
+        <v>146.44999999999999</v>
       </c>
       <c r="K27" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>137.75</v>
+        <v>146.44999999999999</v>
       </c>
       <c r="L27" s="26">
         <f t="shared" ca="1" si="10"/>
-        <v>153.69999999999999</v>
+        <v>134.85</v>
       </c>
       <c r="M27" s="26">
         <f t="shared" ca="1" si="11"/>
-        <v>221.45000000000002</v>
+        <v>219.29999999999998</v>
       </c>
       <c r="N27" s="26">
         <f t="shared" ca="1" si="12"/>
-        <v>148.38333333333333</v>
+        <v>142.58333333333334</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -1980,47 +1980,47 @@
       </c>
       <c r="G29" s="14">
         <f t="shared" ref="G29:N29" ca="1" si="18">SUM(G18:G27)/COUNT(G18:G27)</f>
-        <v>147.28</v>
+        <v>143.375</v>
       </c>
       <c r="H29" s="14">
         <f t="shared" ca="1" si="18"/>
-        <v>153.23000000000002</v>
+        <v>149.61500000000001</v>
       </c>
       <c r="I29" s="14">
         <f t="shared" ca="1" si="18"/>
-        <v>150.70499999999998</v>
+        <v>146.63499999999999</v>
       </c>
       <c r="J29" s="14">
         <f t="shared" ca="1" si="18"/>
-        <v>88.494</v>
+        <v>89.704999999999998</v>
       </c>
       <c r="K29" s="14">
         <f t="shared" ca="1" si="18"/>
-        <v>89.794000000000011</v>
+        <v>86.342000000000013</v>
       </c>
       <c r="L29" s="14">
         <f t="shared" ca="1" si="18"/>
-        <v>86.753999999999991</v>
+        <v>87.935000000000002</v>
       </c>
       <c r="M29" s="14">
         <f t="shared" ca="1" si="18"/>
-        <v>150.40500000000003</v>
+        <v>146.54166666666666</v>
       </c>
       <c r="N29" s="14">
         <f t="shared" ca="1" si="18"/>
-        <v>88.347333333333339</v>
+        <v>87.994</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G30" s="14">
         <f ca="1">SUM(G29:I29) / COUNT(G29:I29)</f>
-        <v>150.405</v>
+        <v>146.54166666666666</v>
       </c>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14">
         <f ca="1">SUM(J29:L29) / COUNT(J29:L29)</f>
-        <v>88.347333333333339</v>
+        <v>87.994000000000014</v>
       </c>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
@@ -2036,7 +2036,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>